<commit_message>
Added Adjacency Tests for Board
</commit_message>
<xml_diff>
--- a/board.xlsx
+++ b/board.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcclu_000\Documents\Classes\CSCI 306\Clue\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="32">
   <si>
     <t>X</t>
   </si>
@@ -102,6 +97,24 @@
   </si>
   <si>
     <t>KR</t>
+  </si>
+  <si>
+    <t>Number of Doors: 18</t>
+  </si>
+  <si>
+    <t>White: Door Direction Tests</t>
+  </si>
+  <si>
+    <t>Orange: Adjacency list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: Adjacency list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: Adjacency lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Pink: walkway scenarios/test targets</t>
   </si>
 </sst>
 </file>
@@ -117,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +161,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -161,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -178,12 +221,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,8 +533,8 @@
     <col min="1" max="27" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -491,7 +555,7 @@
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -552,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -635,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -684,7 +748,7 @@
       <c r="P3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="R3" s="1" t="s">
@@ -718,7 +782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -794,14 +858,14 @@
       <c r="Y4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z4" s="2" t="s">
+      <c r="Z4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="AA4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -820,10 +884,10 @@
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -850,7 +914,7 @@
       <c r="P5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="R5" s="1" t="s">
@@ -884,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -967,8 +1031,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1001,7 +1065,7 @@
       <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -1050,7 +1114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1084,7 +1148,7 @@
       <c r="K8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -1133,7 +1197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1216,7 +1280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1298,8 +1362,9 @@
       <c r="AA10" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD10" s="10"/>
+    </row>
+    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1348,7 +1413,7 @@
       <c r="P11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="11" t="s">
         <v>1</v>
       </c>
       <c r="R11" s="2" t="s">
@@ -1382,7 +1447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1401,7 +1466,7 @@
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1465,7 +1530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1517,10 +1582,10 @@
       <c r="Q13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S13" s="4" t="s">
+      <c r="R13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="T13" s="1" t="s">
@@ -1548,11 +1613,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1631,11 +1696,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1701,7 +1766,7 @@
       <c r="W15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Y15" s="1" t="s">
@@ -1714,7 +1779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1797,7 +1862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1873,14 +1938,15 @@
       <c r="Y17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z17" s="2" t="s">
+      <c r="Z17" s="11" t="s">
         <v>1</v>
       </c>
       <c r="AA17" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH17" s="10"/>
+    </row>
+    <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1899,7 +1965,7 @@
       <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -1923,13 +1989,13 @@
       <c r="N18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="R18" s="2" t="s">
@@ -1944,13 +2010,13 @@
       <c r="U18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X18" s="4" t="s">
+      <c r="X18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="Y18" s="1" t="s">
@@ -1963,7 +2029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2129,7 +2195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2212,7 +2278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2295,7 +2361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2395,7 @@
       <c r="K23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="11" t="s">
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
@@ -2338,7 +2404,7 @@
       <c r="N23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="O23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P23" s="1" t="s">
@@ -2378,7 +2444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -2461,7 +2527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -2544,14 +2610,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -2627,7 +2693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -2707,6 +2773,39 @@
         <v>25</v>
       </c>
       <c r="AA27" s="3"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added target failing tests
</commit_message>
<xml_diff>
--- a/board.xlsx
+++ b/board.xlsx
@@ -529,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>